<commit_message>
Funcionalidad info-reunion a Formato: Funciona también en Colab; BD a formato: mas interactivo y amigable para configurar
</commit_message>
<xml_diff>
--- a/Programación VMC_Septiembre-2024-2025.xlsx
+++ b/Programación VMC_Septiembre-2024-2025.xlsx
@@ -8118,8 +8118,8 @@
     <mergeCell ref="Q25:AC25"/>
     <mergeCell ref="Q3:AC3"/>
     <mergeCell ref="Q21:AC21"/>
+    <mergeCell ref="B25:N25"/>
     <mergeCell ref="Q43:W43"/>
-    <mergeCell ref="B25:N25"/>
     <mergeCell ref="L6:N6"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="B22:H22"/>
@@ -17084,8 +17084,8 @@
     <mergeCell ref="P6:P7"/>
     <mergeCell ref="R6:R7"/>
     <mergeCell ref="D2:D3"/>
+    <mergeCell ref="P2:P3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="P2:P3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="D4:D5"/>
@@ -18247,7 +18247,7 @@
       </c>
       <c r="M11" s="156" t="n"/>
       <c r="N11" s="150" t="n"/>
-      <c r="O11" s="178" t="n"/>
+      <c r="O11" s="178" t="inlineStr"/>
       <c r="P11" s="161" t="n"/>
     </row>
     <row r="12" ht="16.2" customHeight="1" s="167" thickBot="1">
@@ -18261,10 +18261,10 @@
       <c r="I12" s="156" t="n"/>
       <c r="J12" s="156" t="n"/>
       <c r="K12" s="156" t="n"/>
-      <c r="L12" s="162" t="n"/>
+      <c r="L12" s="162" t="inlineStr"/>
       <c r="M12" s="156" t="n"/>
       <c r="N12" s="150" t="n"/>
-      <c r="O12" s="198" t="n"/>
+      <c r="O12" s="198" t="inlineStr"/>
       <c r="P12" s="199" t="n"/>
     </row>
     <row r="13" ht="15" customHeight="1" s="167" thickBot="1">
@@ -18352,7 +18352,7 @@
       <c r="L16" s="156" t="n"/>
       <c r="M16" s="156" t="n"/>
       <c r="N16" s="150" t="n"/>
-      <c r="O16" s="158" t="n"/>
+      <c r="O16" s="158" t="inlineStr"/>
       <c r="P16" s="159" t="n"/>
     </row>
     <row r="17" ht="14.4" customHeight="1" s="167">
@@ -18692,7 +18692,7 @@
       </c>
       <c r="M37" s="156" t="n"/>
       <c r="N37" s="150" t="n"/>
-      <c r="O37" s="178" t="n"/>
+      <c r="O37" s="178" t="inlineStr"/>
       <c r="P37" s="161" t="n"/>
     </row>
     <row r="38" ht="16.2" customHeight="1" s="167" thickBot="1">
@@ -18706,10 +18706,10 @@
       <c r="I38" s="156" t="n"/>
       <c r="J38" s="156" t="n"/>
       <c r="K38" s="156" t="n"/>
-      <c r="L38" s="162" t="n"/>
+      <c r="L38" s="162" t="inlineStr"/>
       <c r="M38" s="156" t="n"/>
       <c r="N38" s="150" t="n"/>
-      <c r="O38" s="198" t="n"/>
+      <c r="O38" s="198" t="inlineStr"/>
       <c r="P38" s="199" t="n"/>
     </row>
     <row r="39" ht="15" customHeight="1" s="167" thickBot="1">
@@ -18797,7 +18797,7 @@
       <c r="L42" s="156" t="n"/>
       <c r="M42" s="156" t="n"/>
       <c r="N42" s="150" t="n"/>
-      <c r="O42" s="158" t="n"/>
+      <c r="O42" s="158" t="inlineStr"/>
       <c r="P42" s="159" t="n"/>
     </row>
     <row r="43" ht="14.4" customHeight="1" s="167">
@@ -23195,7 +23195,6 @@
     <mergeCell ref="O43:P43"/>
     <mergeCell ref="J20:N20"/>
     <mergeCell ref="J52:L52"/>
-    <mergeCell ref="C40:K40"/>
     <mergeCell ref="B76:P76"/>
     <mergeCell ref="O40:P40"/>
     <mergeCell ref="C18:N18"/>
@@ -23236,6 +23235,7 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="L89:N89"/>
     <mergeCell ref="B74:K74"/>
+    <mergeCell ref="C40:K40"/>
     <mergeCell ref="N50:O50"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B6:H6"/>

</xml_diff>